<commit_message>
Test cases for export template
</commit_message>
<xml_diff>
--- a/frappe/core/doctype/data_import/test_data/test_xlsx_raw.xlsx
+++ b/frappe/core/doctype/data_import/test_data/test_xlsx_raw.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Male</t>
   </si>
   <si>
-    <t xml:space="preserve">test0010@gmail.com</t>
+    <t xml:space="preserve">test0100@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Test2</t>
@@ -55,7 +55,7 @@
     <t xml:space="preserve">Kumar</t>
   </si>
   <si>
-    <t xml:space="preserve">test0020@gmail.com</t>
+    <t xml:space="preserve">test0200@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Test3</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Tomar</t>
   </si>
   <si>
-    <t xml:space="preserve">test0030@gmail.com</t>
+    <t xml:space="preserve">test0300@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -179,18 +179,18 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="5:11"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>